<commit_message>
Added a TestFile into branch B
</commit_message>
<xml_diff>
--- a/src/main/java/com/cg/backend_doc_checker/file/TestFile.xlsx
+++ b/src/main/java/com/cg/backend_doc_checker/file/TestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-2025\backend_doc_checker\src\main\java\com\cg\backend_doc_checker\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02105FCB-6B9E-4ADE-9788-6B1A7A3D4B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F337EF-2841-4986-B924-B483813043BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="0" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Hey - I am branch A</t>
+    <t>Hey - I am branch B</t>
   </si>
 </sst>
 </file>
@@ -348,7 +348,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added  I am TestClass in Branch B.
</commit_message>
<xml_diff>
--- a/src/main/java/com/cg/backend_doc_checker/file/TestFile.xlsx
+++ b/src/main/java/com/cg/backend_doc_checker/file/TestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-2025\backend_doc_checker\src\main\java\com\cg\backend_doc_checker\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F337EF-2841-4986-B924-B483813043BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A881C05-DDCE-4084-ACC8-8CD09707048F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="0" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,22 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Hey - I am branch B</t>
   </si>
+  <si>
+    <t>I am TestClass in Branch B.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,8 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,20 +357,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>